<commit_message>
finished week 1 analysis
</commit_message>
<xml_diff>
--- a/Bulk Program.xlsx
+++ b/Bulk Program.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adcsuf-my.sharepoint.com/personal/arman714_csu_fullerton_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adcsuf-my.sharepoint.com/personal/arman714_csu_fullerton_edu/Documents/Personal Coding/Bulk Program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{5BDB173E-0807-3D46-9148-FEADD902EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4D53DDA-62D7-46CA-870E-C508012D7799}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{5BDB173E-0807-3D46-9148-FEADD902EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F19AB7A-24A9-4019-9A59-BE8BC8716812}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{08254556-42EC-6440-87DE-94FC0AA2B1AD}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{08254556-42EC-6440-87DE-94FC0AA2B1AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance" sheetId="1" r:id="rId1"/>
@@ -36,38 +36,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
-  <si>
-    <t>Flat Bench Press</t>
-  </si>
-  <si>
-    <t>Chest Fly</t>
-  </si>
-  <si>
-    <t>Incline Machine Press</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Tricep Extension</t>
   </si>
   <si>
-    <t>Lateral Raise</t>
-  </si>
-  <si>
     <t>Barbell Curl</t>
   </si>
   <si>
     <t>Lat Pulldown</t>
   </si>
   <si>
-    <t>Seated Row</t>
-  </si>
-  <si>
     <t>Hammer Curl</t>
   </si>
   <si>
-    <t>Rear Delt</t>
-  </si>
-  <si>
     <t>Hamstring Curl</t>
   </si>
   <si>
@@ -80,24 +62,12 @@
     <t>Tricep Dips</t>
   </si>
   <si>
-    <t>Shoulder Press</t>
-  </si>
-  <si>
-    <t>Flat Machine Press</t>
-  </si>
-  <si>
     <t>Cable Fly</t>
   </si>
   <si>
     <t>T Bar Row</t>
   </si>
   <si>
-    <t>Pull ups</t>
-  </si>
-  <si>
-    <t>Bicep curl</t>
-  </si>
-  <si>
     <t>Chest</t>
   </si>
   <si>
@@ -116,9 +86,6 @@
     <t>Legs</t>
   </si>
   <si>
-    <t>Bicep Curl</t>
-  </si>
-  <si>
     <t>Skull Crusher</t>
   </si>
   <si>
@@ -156,6 +123,42 @@
   </si>
   <si>
     <t>Day 5 - Pull, Tris, Shoulder</t>
+  </si>
+  <si>
+    <t>Barbell Bench Press</t>
+  </si>
+  <si>
+    <t>Cable Curl</t>
+  </si>
+  <si>
+    <t>Machine Fly</t>
+  </si>
+  <si>
+    <t>Dumbbell Curl</t>
+  </si>
+  <si>
+    <t>Pull Ups</t>
+  </si>
+  <si>
+    <t>Face Pull</t>
+  </si>
+  <si>
+    <t>Cable Lateral Raise</t>
+  </si>
+  <si>
+    <t>Dumbbell Lateral Raise</t>
+  </si>
+  <si>
+    <t>Barbell Overhead Press</t>
+  </si>
+  <si>
+    <t>Incline Press</t>
+  </si>
+  <si>
+    <t>Flat Press</t>
+  </si>
+  <si>
+    <t>Cable Row</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,7 +774,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -793,37 +792,37 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B1" s="25"/>
       <c r="D1" s="26" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E3" s="17">
         <v>2</v>
@@ -831,13 +830,13 @@
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" s="18">
         <v>2</v>
@@ -845,13 +844,13 @@
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E5" s="18">
         <v>2</v>
@@ -859,13 +858,13 @@
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B6" s="9">
         <v>2</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E6" s="9">
         <v>2</v>
@@ -873,13 +872,13 @@
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B7" s="11">
         <v>2</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E7" s="9">
         <v>2</v>
@@ -887,13 +886,13 @@
     </row>
     <row r="8" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E8" s="19">
         <v>2</v>
@@ -917,41 +916,41 @@
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="24" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="1"/>
       <c r="D11" s="24" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E11" s="25"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="20" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B13" s="21">
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
@@ -961,13 +960,13 @@
     </row>
     <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="20" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B14" s="21">
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7">
         <v>2</v>
@@ -977,13 +976,13 @@
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="20" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B15" s="21">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
@@ -992,13 +991,13 @@
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>3</v>
-      </c>
-      <c r="B16" s="9">
-        <v>2</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="E16" s="17">
         <v>2</v>
@@ -1009,13 +1008,13 @@
     </row>
     <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B17" s="11">
         <v>2</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="E17" s="11">
         <v>2</v>
@@ -1026,13 +1025,13 @@
     </row>
     <row r="18" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="22" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B18" s="23">
         <v>2</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E18" s="19">
         <v>2</v>
@@ -1058,25 +1057,25 @@
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="24" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B21" s="25"/>
       <c r="D21" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E22" s="7">
         <v>6</v>
@@ -1084,13 +1083,13 @@
     </row>
     <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B23" s="11">
         <v>2</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E23" s="9">
         <v>5</v>
@@ -1098,13 +1097,13 @@
     </row>
     <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B24" s="18">
         <v>2</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E24" s="17">
         <v>4</v>
@@ -1112,13 +1111,13 @@
     </row>
     <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B25" s="18">
         <v>2</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E25" s="11">
         <v>5</v>
@@ -1126,13 +1125,13 @@
     </row>
     <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="14" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B26" s="17">
         <v>2</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E26" s="18">
         <v>4</v>
@@ -1140,13 +1139,13 @@
     </row>
     <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B27" s="9">
         <v>2</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E27" s="21">
         <v>3</v>
@@ -1154,13 +1153,13 @@
     </row>
     <row r="28" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B28" s="19">
         <v>2</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E28" s="19">
         <v>3</v>

</xml_diff>

<commit_message>
parsed ordered_dicts and wrote to excel
</commit_message>
<xml_diff>
--- a/Bulk Program.xlsx
+++ b/Bulk Program.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adcsuf-my.sharepoint.com/personal/arman714_csu_fullerton_edu/Documents/Personal Coding/Bulk Program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{5BDB173E-0807-3D46-9148-FEADD902EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F19AB7A-24A9-4019-9A59-BE8BC8716812}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{5BDB173E-0807-3D46-9148-FEADD902EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{950FD90B-1776-40A3-8310-D5178930AC55}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{08254556-42EC-6440-87DE-94FC0AA2B1AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{08254556-42EC-6440-87DE-94FC0AA2B1AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Maintenance" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Tricep Extension</t>
   </si>
@@ -159,13 +159,37 @@
   </si>
   <si>
     <t>Cable Row</t>
+  </si>
+  <si>
+    <t>Day 6 - Back, Hams, Accessories (Optional)</t>
+  </si>
+  <si>
+    <t>Deadlift</t>
+  </si>
+  <si>
+    <t>5 Day Total</t>
+  </si>
+  <si>
+    <t>6 Day Total</t>
+  </si>
+  <si>
+    <t>Preacher Curl / Hammer Curl</t>
+  </si>
+  <si>
+    <t>Tricep Dips / Tricep Extension</t>
+  </si>
+  <si>
+    <t>Dumbbell / Cable / Iso Lateral Raise</t>
+  </si>
+  <si>
+    <t>Calf Raise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +208,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -356,6 +386,32 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -432,12 +488,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,6 +498,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -472,6 +528,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -771,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4378B549-3B91-3546-81EA-BAF64B222B94}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -791,14 +851,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="D1" s="26" t="s">
+      <c r="B1" s="23"/>
+      <c r="D1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
@@ -915,15 +975,15 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="23"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.4">
@@ -972,7 +1032,6 @@
         <v>2</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="20" t="s">
@@ -990,10 +1049,10 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="9">
+      <c r="A16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="11">
         <v>2</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -1007,10 +1066,10 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="11">
+      <c r="A17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="9">
         <v>2</v>
       </c>
       <c r="D17" s="10" t="s">
@@ -1024,10 +1083,10 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="23">
+      <c r="A18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="11">
         <v>2</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -1060,12 +1119,10 @@
         <v>28</v>
       </c>
       <c r="B21" s="25"/>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D21" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
@@ -1074,11 +1131,11 @@
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="7">
-        <v>6</v>
+      <c r="D22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.4">
@@ -1088,11 +1145,11 @@
       <c r="B23" s="11">
         <v>2</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="9">
-        <v>5</v>
+      <c r="D23" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="21">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.4">
@@ -1102,11 +1159,11 @@
       <c r="B24" s="18">
         <v>2</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="17">
-        <v>4</v>
+      <c r="D24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.4">
@@ -1116,39 +1173,39 @@
       <c r="B25" s="18">
         <v>2</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="11">
-        <v>5</v>
+      <c r="D25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="9">
+        <v>2</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A27" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="17">
-        <v>2</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="9">
+      <c r="B27" s="17">
         <v>2</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="E27" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -1162,17 +1219,144 @@
         <v>17</v>
       </c>
       <c r="E28" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="D31" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="7">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="9">
+        <v>5</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="17">
+        <v>4</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="11">
+        <v>5</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A37" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="18">
+        <v>4</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A38" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="21">
         <v>3</v>
       </c>
+      <c r="D38" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="19">
+        <v>3</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="19">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D21:E21"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>